<commit_message>
GEP00010 project submission repaired
</commit_message>
<xml_diff>
--- a/data/GEP00010/GEP00010.xlsx
+++ b/data/GEP00010/GEP00010.xlsx
@@ -18,10 +18,8 @@
     <sheet name="SequencingLibrary" sheetId="8" r:id="rId9"/>
     <sheet name="Menus" sheetId="9" r:id="rId10"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId11"/>
-  </externalReferences>
   <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -2572,13 +2570,13 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="41" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="42" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="134">
     <cellStyle name="20% - 着色 1 2" xfId="101"/>
@@ -3146,19 +3144,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Menus]\Users\pajon01\workspace\genome"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:C13" totalsRowShown="0">
   <tableColumns count="3">
@@ -3584,18 +3569,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="23" thickBot="1">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>166</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
     </row>
     <row r="2" spans="1:3" ht="21" thickTop="1" thickBot="1">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
     </row>
     <row r="3" spans="1:3" ht="18" thickTop="1">
       <c r="A3" s="4" t="s">
@@ -4772,28 +4757,6 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Menus!$C$2:$C$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>H4:H1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Menus!$B$2:$B$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>C5:C1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>'[1]Menus]\Users\pajon01\workspace\genome'!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>C2:C4</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
@@ -5255,7 +5218,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J7" sqref="J7:L7"/>
     </sheetView>
   </sheetViews>
@@ -5418,13 +5381,13 @@
       <c r="I3" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="J3" s="14" t="s">
         <v>267</v>
       </c>
-      <c r="K3" s="16" t="s">
+      <c r="K3" s="14" t="s">
         <v>480</v>
       </c>
-      <c r="L3" s="16" t="s">
+      <c r="L3" s="14" t="s">
         <v>481</v>
       </c>
       <c r="M3" s="2" t="s">

</xml_diff>

<commit_message>
update primer locations for GEP00010
</commit_message>
<xml_diff>
--- a/data/GEP00010/GEP00010.xlsx
+++ b/data/GEP00010/GEP00010.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr updateLinks="never" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="31080" windowHeight="13520" tabRatio="736" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33580" windowHeight="13520" tabRatio="736" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Documentation" sheetId="10" r:id="rId1"/>
@@ -18,8 +18,7 @@
     <sheet name="SequencingLibrary" sheetId="8" r:id="rId9"/>
     <sheet name="Menus" sheetId="9" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1545" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1543" uniqueCount="480">
   <si>
     <t>geid</t>
   </si>
@@ -1917,12 +1916,6 @@
   <si>
     <t>CCKAR.1</t>
     <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>65637077</t>
-  </si>
-  <si>
-    <t>65637096</t>
   </si>
 </sst>
 </file>
@@ -2419,7 +2412,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="134">
+  <cellStyleXfs count="172">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2554,8 +2547,46 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -2570,15 +2601,16 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="41" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="42" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="134">
+  <cellStyles count="172">
     <cellStyle name="20% - 着色 1 2" xfId="101"/>
     <cellStyle name="20% - 着色 2 2" xfId="105"/>
     <cellStyle name="20% - 着色 3 2" xfId="109"/>
@@ -2641,6 +2673,25 @@
     <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="143" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="145" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="147" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="149" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="151" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="153" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="155" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="157" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="159" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="161" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="163" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="165" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="167" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="169" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="171" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="42" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -2686,6 +2737,25 @@
     <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="134" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="136" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="138" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="140" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="142" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="144" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="146" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="148" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="150" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="152" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="154" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="156" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="158" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="160" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="162" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="164" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="166" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="168" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="170" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="124"/>
     <cellStyle name="Normal 3" xfId="126"/>
@@ -3569,18 +3639,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="23" thickBot="1">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
     </row>
     <row r="2" spans="1:3" ht="21" thickTop="1" thickBot="1">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
     </row>
     <row r="3" spans="1:3" ht="18" thickTop="1">
       <c r="A3" s="4" t="s">
@@ -5216,10 +5286,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R7"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7:L7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -5353,117 +5423,112 @@
       </c>
       <c r="R2" s="2"/>
     </row>
-    <row r="3" spans="1:18">
-      <c r="A3" t="s">
+    <row r="3" spans="1:18" s="16" customFormat="1">
+      <c r="A3" s="16" t="s">
         <v>478</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="16" t="s">
         <v>251</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="16">
         <v>65637008</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="11" t="s">
         <v>252</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="11" t="s">
         <v>256</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="J3" s="17" t="s">
         <v>267</v>
       </c>
-      <c r="K3" s="14" t="s">
-        <v>480</v>
-      </c>
-      <c r="L3" s="14" t="s">
-        <v>481</v>
-      </c>
-      <c r="M3" s="2" t="s">
+      <c r="K3" s="16">
+        <v>65636864</v>
+      </c>
+      <c r="L3" s="16">
+        <v>65636884</v>
+      </c>
+      <c r="M3" s="11" t="s">
         <v>257</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="N3" s="11" t="s">
         <v>266</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="O3" s="11" t="s">
         <v>264</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="P3" s="11" t="s">
         <v>265</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="Q3" s="11" t="s">
         <v>189</v>
       </c>
-      <c r="R3" s="2"/>
-    </row>
-    <row r="4" spans="1:18">
-      <c r="A4" t="s">
+      <c r="R3" s="11"/>
+    </row>
+    <row r="4" spans="1:18" s="16" customFormat="1">
+      <c r="A4" s="16" t="s">
         <v>479</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="16" t="s">
         <v>251</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="16">
         <v>26481627</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="11" t="s">
         <v>256</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="11">
         <v>4</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="11" t="s">
         <v>258</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="16" t="s">
         <v>260</v>
       </c>
-      <c r="K4" s="2">
-        <v>26481482</v>
-      </c>
-      <c r="L4" s="2">
-        <v>26481500</v>
-      </c>
-      <c r="M4" s="2" t="s">
+      <c r="K4" s="16">
+        <v>26481536</v>
+      </c>
+      <c r="L4" s="16">
+        <v>26481556</v>
+      </c>
+      <c r="M4" s="11" t="s">
         <v>259</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" s="16" t="s">
         <v>261</v>
       </c>
-      <c r="O4" s="2">
-        <v>26481710</v>
-      </c>
-      <c r="P4" s="2">
-        <v>26481729</v>
-      </c>
-      <c r="Q4" s="2" t="s">
+      <c r="O4" s="16">
+        <v>26481765</v>
+      </c>
+      <c r="P4" s="16">
+        <v>26481784</v>
+      </c>
+      <c r="Q4" s="11" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="7" spans="1:18">
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="11" type="noConversion"/>
@@ -8300,7 +8365,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G133"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E88" sqref="E88"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update primer coordinates for GEP00010 and modify script to take into account guide strand
</commit_message>
<xml_diff>
--- a/data/GEP00010/GEP00010.xlsx
+++ b/data/GEP00010/GEP00010.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr updateLinks="never" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33580" windowHeight="13520" tabRatio="736" activeTab="5"/>
+    <workbookView xWindow="-60" yWindow="5500" windowWidth="33580" windowHeight="13520" tabRatio="736" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Documentation" sheetId="10" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1543" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1541" uniqueCount="478">
   <si>
     <t>geid</t>
   </si>
@@ -1053,14 +1053,6 @@
   </si>
   <si>
     <t>CCA</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>65637123</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>65637142</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
@@ -2412,7 +2404,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="172">
+  <cellStyleXfs count="174">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2585,6 +2577,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2601,16 +2595,16 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="41" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="42" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="172">
+  <cellStyles count="174">
     <cellStyle name="20% - 着色 1 2" xfId="101"/>
     <cellStyle name="20% - 着色 2 2" xfId="105"/>
     <cellStyle name="20% - 着色 3 2" xfId="109"/>
@@ -2692,6 +2686,7 @@
     <cellStyle name="Followed Hyperlink" xfId="167" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="169" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="171" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="173" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="42" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -2756,6 +2751,7 @@
     <cellStyle name="Hyperlink" xfId="166" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="168" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="170" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="172" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="124"/>
     <cellStyle name="Normal 3" xfId="126"/>
@@ -3639,18 +3635,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="23" thickBot="1">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>166</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
     </row>
     <row r="2" spans="1:3" ht="21" thickTop="1" thickBot="1">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
     </row>
     <row r="3" spans="1:3" ht="18" thickTop="1">
       <c r="A3" s="4" t="s">
@@ -4632,7 +4628,7 @@
         <v>236</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>173</v>
@@ -4653,7 +4649,7 @@
         <v>234</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="J2" s="9"/>
     </row>
@@ -5289,7 +5285,7 @@
   <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -5371,7 +5367,7 @@
     </row>
     <row r="2" spans="1:18">
       <c r="A2" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B2" t="s">
         <v>234</v>
@@ -5400,10 +5396,10 @@
       <c r="J2" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2">
         <v>53704130</v>
       </c>
-      <c r="L2" s="2">
+      <c r="L2">
         <v>53704148</v>
       </c>
       <c r="M2" s="11" t="s">
@@ -5412,10 +5408,10 @@
       <c r="N2" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="O2" s="2">
+      <c r="O2">
         <v>53704291</v>
       </c>
-      <c r="P2" s="2">
+      <c r="P2">
         <v>53704310</v>
       </c>
       <c r="Q2" s="2" t="s">
@@ -5423,18 +5419,18 @@
       </c>
       <c r="R2" s="2"/>
     </row>
-    <row r="3" spans="1:18" s="16" customFormat="1">
-      <c r="A3" s="16" t="s">
-        <v>478</v>
-      </c>
-      <c r="B3" s="16" t="s">
+    <row r="3" spans="1:18" s="14" customFormat="1">
+      <c r="A3" s="14" t="s">
+        <v>476</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>251</v>
       </c>
-      <c r="C3" s="16">
+      <c r="C3" s="14">
         <v>65637008</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>252</v>
+        <v>58</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>256</v>
@@ -5451,40 +5447,40 @@
       <c r="I3" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="J3" s="17" t="s">
-        <v>267</v>
-      </c>
-      <c r="K3" s="16">
+      <c r="J3" s="15" t="s">
+        <v>265</v>
+      </c>
+      <c r="K3">
         <v>65636864</v>
       </c>
-      <c r="L3" s="16">
-        <v>65636884</v>
+      <c r="L3">
+        <v>65636883</v>
       </c>
       <c r="M3" s="11" t="s">
         <v>257</v>
       </c>
       <c r="N3" s="11" t="s">
-        <v>266</v>
-      </c>
-      <c r="O3" s="11" t="s">
         <v>264</v>
       </c>
-      <c r="P3" s="11" t="s">
-        <v>265</v>
+      <c r="O3">
+        <v>65637077</v>
+      </c>
+      <c r="P3">
+        <v>65637096</v>
       </c>
       <c r="Q3" s="11" t="s">
         <v>189</v>
       </c>
       <c r="R3" s="11"/>
     </row>
-    <row r="4" spans="1:18" s="16" customFormat="1">
-      <c r="A4" s="16" t="s">
-        <v>479</v>
-      </c>
-      <c r="B4" s="16" t="s">
+    <row r="4" spans="1:18" s="14" customFormat="1">
+      <c r="A4" s="14" t="s">
+        <v>477</v>
+      </c>
+      <c r="B4" s="14" t="s">
         <v>251</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4" s="14">
         <v>26481627</v>
       </c>
       <c r="D4" s="11" t="s">
@@ -5505,25 +5501,25 @@
       <c r="I4" s="11" t="s">
         <v>258</v>
       </c>
-      <c r="J4" s="16" t="s">
+      <c r="J4" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="K4" s="16">
-        <v>26481536</v>
-      </c>
-      <c r="L4" s="16">
+      <c r="K4">
+        <v>26481537</v>
+      </c>
+      <c r="L4">
         <v>26481556</v>
       </c>
       <c r="M4" s="11" t="s">
         <v>259</v>
       </c>
-      <c r="N4" s="16" t="s">
+      <c r="N4" s="14" t="s">
         <v>261</v>
       </c>
-      <c r="O4" s="16">
-        <v>26481765</v>
-      </c>
-      <c r="P4" s="16">
+      <c r="O4">
+        <v>26481766</v>
+      </c>
+      <c r="P4">
         <v>26481784</v>
       </c>
       <c r="Q4" s="11" t="s">
@@ -5627,10 +5623,10 @@
         <v>236</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>172</v>
@@ -5657,10 +5653,10 @@
         <v>236</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>172</v>
@@ -5687,10 +5683,10 @@
         <v>236</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>172</v>
@@ -5717,10 +5713,10 @@
         <v>236</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>172</v>
@@ -5747,16 +5743,16 @@
         <v>236</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>172</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G6" t="s">
         <v>245</v>
@@ -5777,16 +5773,16 @@
         <v>236</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>172</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G7" t="s">
         <v>245</v>
@@ -5807,16 +5803,16 @@
         <v>236</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>172</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G8" t="s">
         <v>245</v>
@@ -5837,16 +5833,16 @@
         <v>236</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>172</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G9" t="s">
         <v>245</v>
@@ -5867,16 +5863,16 @@
         <v>236</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>172</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G10" t="s">
         <v>247</v>
@@ -5897,16 +5893,16 @@
         <v>236</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>172</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G11" t="s">
         <v>247</v>
@@ -5927,16 +5923,16 @@
         <v>236</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>172</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G12" t="s">
         <v>247</v>
@@ -5957,16 +5953,16 @@
         <v>236</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D13" s="12" t="s">
         <v>172</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G13" t="s">
         <v>247</v>
@@ -5987,10 +5983,10 @@
         <v>236</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>172</v>
@@ -6017,10 +6013,10 @@
         <v>236</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>172</v>
@@ -6047,10 +6043,10 @@
         <v>236</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>172</v>
@@ -6077,10 +6073,10 @@
         <v>236</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D17" s="12" t="s">
         <v>172</v>
@@ -6107,16 +6103,16 @@
         <v>236</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D18" s="12" t="s">
         <v>172</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G18" t="s">
         <v>245</v>
@@ -6137,16 +6133,16 @@
         <v>236</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D19" s="12" t="s">
         <v>172</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G19" t="s">
         <v>245</v>
@@ -6167,16 +6163,16 @@
         <v>236</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D20" s="12" t="s">
         <v>172</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G20" t="s">
         <v>245</v>
@@ -6197,16 +6193,16 @@
         <v>236</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D21" s="12" t="s">
         <v>172</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G21" t="s">
         <v>245</v>
@@ -6227,16 +6223,16 @@
         <v>236</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D22" s="12" t="s">
         <v>172</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G22" t="s">
         <v>247</v>
@@ -6257,16 +6253,16 @@
         <v>236</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D23" s="12" t="s">
         <v>172</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G23" t="s">
         <v>247</v>
@@ -6287,16 +6283,16 @@
         <v>236</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D24" s="12" t="s">
         <v>172</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G24" t="s">
         <v>247</v>
@@ -6317,16 +6313,16 @@
         <v>236</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D25" s="12" t="s">
         <v>172</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G25" t="s">
         <v>247</v>
@@ -6347,10 +6343,10 @@
         <v>236</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D26" s="12" t="s">
         <v>172</v>
@@ -6377,10 +6373,10 @@
         <v>236</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D27" s="12" t="s">
         <v>172</v>
@@ -6407,10 +6403,10 @@
         <v>236</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D28" s="12" t="s">
         <v>172</v>
@@ -6437,10 +6433,10 @@
         <v>236</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D29" s="12" t="s">
         <v>172</v>
@@ -6467,16 +6463,16 @@
         <v>236</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D30" s="12" t="s">
         <v>172</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G30" t="s">
         <v>245</v>
@@ -6497,16 +6493,16 @@
         <v>236</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D31" s="12" t="s">
         <v>172</v>
       </c>
       <c r="F31" s="12" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G31" t="s">
         <v>245</v>
@@ -6527,16 +6523,16 @@
         <v>236</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D32" s="12" t="s">
         <v>172</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G32" t="s">
         <v>245</v>
@@ -6557,16 +6553,16 @@
         <v>236</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D33" s="12" t="s">
         <v>172</v>
       </c>
       <c r="F33" s="12" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G33" t="s">
         <v>245</v>
@@ -6587,16 +6583,16 @@
         <v>236</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D34" s="12" t="s">
         <v>172</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G34" t="s">
         <v>247</v>
@@ -6617,16 +6613,16 @@
         <v>236</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D35" s="12" t="s">
         <v>172</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G35" t="s">
         <v>247</v>
@@ -6647,16 +6643,16 @@
         <v>236</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D36" s="12" t="s">
         <v>172</v>
       </c>
       <c r="F36" s="12" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G36" t="s">
         <v>247</v>
@@ -6677,16 +6673,16 @@
         <v>236</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D37" s="12" t="s">
         <v>172</v>
       </c>
       <c r="F37" s="12" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G37" t="s">
         <v>247</v>
@@ -6707,7 +6703,7 @@
         <v>236</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C38" s="12" t="s">
         <v>198</v>
@@ -6737,7 +6733,7 @@
         <v>236</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C39" s="12" t="s">
         <v>199</v>
@@ -6767,7 +6763,7 @@
         <v>236</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C40" s="12" t="s">
         <v>200</v>
@@ -6797,7 +6793,7 @@
         <v>236</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C41" s="12" t="s">
         <v>201</v>
@@ -6827,7 +6823,7 @@
         <v>236</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C42" s="12" t="s">
         <v>202</v>
@@ -6836,7 +6832,7 @@
         <v>172</v>
       </c>
       <c r="F42" s="12" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G42" t="s">
         <v>245</v>
@@ -6857,7 +6853,7 @@
         <v>236</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C43" s="12" t="s">
         <v>203</v>
@@ -6866,7 +6862,7 @@
         <v>172</v>
       </c>
       <c r="F43" s="12" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G43" t="s">
         <v>245</v>
@@ -6887,7 +6883,7 @@
         <v>236</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C44" s="12" t="s">
         <v>204</v>
@@ -6896,7 +6892,7 @@
         <v>172</v>
       </c>
       <c r="F44" s="12" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G44" t="s">
         <v>245</v>
@@ -6917,7 +6913,7 @@
         <v>236</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C45" s="12" t="s">
         <v>205</v>
@@ -6926,7 +6922,7 @@
         <v>172</v>
       </c>
       <c r="F45" s="12" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G45" t="s">
         <v>245</v>
@@ -6947,7 +6943,7 @@
         <v>236</v>
       </c>
       <c r="B46" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C46" s="12" t="s">
         <v>206</v>
@@ -6956,7 +6952,7 @@
         <v>172</v>
       </c>
       <c r="F46" s="12" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G46" t="s">
         <v>247</v>
@@ -6977,7 +6973,7 @@
         <v>236</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C47" s="12" t="s">
         <v>207</v>
@@ -6986,7 +6982,7 @@
         <v>172</v>
       </c>
       <c r="F47" s="12" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G47" t="s">
         <v>247</v>
@@ -7007,7 +7003,7 @@
         <v>236</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C48" s="12" t="s">
         <v>208</v>
@@ -7016,7 +7012,7 @@
         <v>172</v>
       </c>
       <c r="F48" s="12" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G48" t="s">
         <v>247</v>
@@ -7037,7 +7033,7 @@
         <v>236</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C49" s="12" t="s">
         <v>209</v>
@@ -7046,7 +7042,7 @@
         <v>172</v>
       </c>
       <c r="F49" s="12" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G49" t="s">
         <v>247</v>
@@ -7067,7 +7063,7 @@
         <v>236</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C50" s="12" t="s">
         <v>210</v>
@@ -7097,7 +7093,7 @@
         <v>236</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C51" s="12" t="s">
         <v>211</v>
@@ -7127,7 +7123,7 @@
         <v>236</v>
       </c>
       <c r="B52" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C52" s="12" t="s">
         <v>212</v>
@@ -7157,7 +7153,7 @@
         <v>236</v>
       </c>
       <c r="B53" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C53" s="12" t="s">
         <v>213</v>
@@ -7187,7 +7183,7 @@
         <v>236</v>
       </c>
       <c r="B54" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C54" s="12" t="s">
         <v>214</v>
@@ -7196,7 +7192,7 @@
         <v>172</v>
       </c>
       <c r="F54" s="12" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G54" t="s">
         <v>245</v>
@@ -7217,7 +7213,7 @@
         <v>236</v>
       </c>
       <c r="B55" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C55" s="12" t="s">
         <v>215</v>
@@ -7226,7 +7222,7 @@
         <v>172</v>
       </c>
       <c r="F55" s="12" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G55" t="s">
         <v>245</v>
@@ -7247,7 +7243,7 @@
         <v>236</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C56" s="12" t="s">
         <v>216</v>
@@ -7256,7 +7252,7 @@
         <v>172</v>
       </c>
       <c r="F56" s="12" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G56" t="s">
         <v>245</v>
@@ -7277,7 +7273,7 @@
         <v>236</v>
       </c>
       <c r="B57" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C57" s="12" t="s">
         <v>217</v>
@@ -7286,7 +7282,7 @@
         <v>172</v>
       </c>
       <c r="F57" s="12" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G57" t="s">
         <v>245</v>
@@ -7307,7 +7303,7 @@
         <v>236</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C58" s="12" t="s">
         <v>218</v>
@@ -7316,7 +7312,7 @@
         <v>172</v>
       </c>
       <c r="F58" s="12" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G58" t="s">
         <v>247</v>
@@ -7337,7 +7333,7 @@
         <v>236</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C59" s="12" t="s">
         <v>219</v>
@@ -7346,7 +7342,7 @@
         <v>172</v>
       </c>
       <c r="F59" s="12" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G59" t="s">
         <v>247</v>
@@ -7367,7 +7363,7 @@
         <v>236</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C60" s="12" t="s">
         <v>220</v>
@@ -7376,7 +7372,7 @@
         <v>172</v>
       </c>
       <c r="F60" s="12" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G60" t="s">
         <v>247</v>
@@ -7397,7 +7393,7 @@
         <v>236</v>
       </c>
       <c r="B61" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C61" s="12" t="s">
         <v>221</v>
@@ -7406,7 +7402,7 @@
         <v>172</v>
       </c>
       <c r="F61" s="12" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G61" t="s">
         <v>247</v>
@@ -7427,7 +7423,7 @@
         <v>236</v>
       </c>
       <c r="B62" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C62" s="12" t="s">
         <v>222</v>
@@ -7457,7 +7453,7 @@
         <v>236</v>
       </c>
       <c r="B63" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C63" s="12" t="s">
         <v>223</v>
@@ -7487,7 +7483,7 @@
         <v>236</v>
       </c>
       <c r="B64" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C64" s="12" t="s">
         <v>224</v>
@@ -7517,7 +7513,7 @@
         <v>236</v>
       </c>
       <c r="B65" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C65" s="12" t="s">
         <v>225</v>
@@ -7547,7 +7543,7 @@
         <v>236</v>
       </c>
       <c r="B66" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C66" s="12" t="s">
         <v>226</v>
@@ -7556,7 +7552,7 @@
         <v>172</v>
       </c>
       <c r="F66" s="12" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G66" t="s">
         <v>245</v>
@@ -7577,7 +7573,7 @@
         <v>236</v>
       </c>
       <c r="B67" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C67" s="12" t="s">
         <v>227</v>
@@ -7586,7 +7582,7 @@
         <v>172</v>
       </c>
       <c r="F67" s="12" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G67" t="s">
         <v>245</v>
@@ -7607,7 +7603,7 @@
         <v>236</v>
       </c>
       <c r="B68" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C68" s="12" t="s">
         <v>228</v>
@@ -7616,7 +7612,7 @@
         <v>172</v>
       </c>
       <c r="F68" s="12" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G68" t="s">
         <v>245</v>
@@ -7637,7 +7633,7 @@
         <v>236</v>
       </c>
       <c r="B69" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C69" s="12" t="s">
         <v>229</v>
@@ -7646,7 +7642,7 @@
         <v>172</v>
       </c>
       <c r="F69" s="12" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G69" t="s">
         <v>245</v>
@@ -7667,7 +7663,7 @@
         <v>236</v>
       </c>
       <c r="B70" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C70" s="12" t="s">
         <v>230</v>
@@ -7676,7 +7672,7 @@
         <v>172</v>
       </c>
       <c r="F70" s="12" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G70" t="s">
         <v>247</v>
@@ -7697,7 +7693,7 @@
         <v>236</v>
       </c>
       <c r="B71" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C71" s="12" t="s">
         <v>231</v>
@@ -7706,7 +7702,7 @@
         <v>172</v>
       </c>
       <c r="F71" s="12" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G71" t="s">
         <v>247</v>
@@ -7727,7 +7723,7 @@
         <v>236</v>
       </c>
       <c r="B72" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C72" s="12" t="s">
         <v>232</v>
@@ -7736,7 +7732,7 @@
         <v>172</v>
       </c>
       <c r="F72" s="12" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G72" t="s">
         <v>247</v>
@@ -7757,7 +7753,7 @@
         <v>236</v>
       </c>
       <c r="B73" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C73" s="12" t="s">
         <v>233</v>
@@ -7766,7 +7762,7 @@
         <v>172</v>
       </c>
       <c r="F73" s="12" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G73" t="s">
         <v>247</v>
@@ -7787,16 +7783,16 @@
         <v>236</v>
       </c>
       <c r="B74" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C74" s="12" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D74" s="12" t="s">
         <v>172</v>
       </c>
       <c r="F74" s="12" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G74" t="s">
         <v>247</v>
@@ -7817,10 +7813,10 @@
         <v>236</v>
       </c>
       <c r="B75" s="13" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C75" s="12" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D75" s="12" t="s">
         <v>172</v>
@@ -7847,10 +7843,10 @@
         <v>236</v>
       </c>
       <c r="B76" s="13" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C76" s="12" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D76" s="12" t="s">
         <v>172</v>
@@ -7877,10 +7873,10 @@
         <v>236</v>
       </c>
       <c r="B77" s="13" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C77" s="12" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D77" s="12" t="s">
         <v>172</v>
@@ -7907,10 +7903,10 @@
         <v>236</v>
       </c>
       <c r="B78" s="13" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C78" s="12" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D78" s="12" t="s">
         <v>172</v>
@@ -7937,10 +7933,10 @@
         <v>236</v>
       </c>
       <c r="B79" s="13" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C79" s="12" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D79" s="12" t="s">
         <v>172</v>
@@ -7967,10 +7963,10 @@
         <v>236</v>
       </c>
       <c r="B80" s="13" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C80" s="12" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D80" s="12" t="s">
         <v>172</v>
@@ -7997,10 +7993,10 @@
         <v>236</v>
       </c>
       <c r="B81" s="13" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C81" s="12" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D81" s="12" t="s">
         <v>172</v>
@@ -8027,10 +8023,10 @@
         <v>236</v>
       </c>
       <c r="B82" s="13" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C82" s="12" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D82" s="12" t="s">
         <v>172</v>
@@ -8057,10 +8053,10 @@
         <v>236</v>
       </c>
       <c r="B83" s="13" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C83" s="12" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D83" s="12" t="s">
         <v>172</v>
@@ -8305,13 +8301,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D2" t="s">
         <v>191</v>
@@ -8319,13 +8315,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B3" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C3" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D3" t="s">
         <v>191</v>
@@ -8333,13 +8329,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B4" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C4" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D4" t="s">
         <v>191</v>
@@ -8403,22 +8399,22 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>71</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E2" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="G2" s="12" t="s">
         <v>192</v>
@@ -8426,68 +8422,68 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>71</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E3" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>71</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>71</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="G5" s="12" t="s">
         <v>193</v>
@@ -8495,482 +8491,482 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>71</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E6" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>71</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>71</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>71</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>71</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E10" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>71</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E11" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>71</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E12" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>71</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E13" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>71</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E14" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C15" s="13" t="s">
         <v>71</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E15" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C16" s="13" t="s">
         <v>71</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E16" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C17" s="13" t="s">
         <v>71</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E17" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C18" s="13" t="s">
         <v>71</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E18" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C19" s="13" t="s">
         <v>71</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E19" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C20" s="13" t="s">
         <v>71</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E20" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>71</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E21" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C22" s="13" t="s">
         <v>71</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E22" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>71</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E23" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C24" s="13" t="s">
         <v>71</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E24" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C25" s="13" t="s">
         <v>71</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E25" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="G25" s="12" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C26" s="13" t="s">
         <v>71</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E26" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="G26" s="12" t="s">
         <v>194</v>
@@ -8978,22 +8974,22 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C27" s="13" t="s">
         <v>71</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E27" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="G27" s="12" t="s">
         <v>195</v>
@@ -9001,22 +8997,22 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C28" s="13" t="s">
         <v>71</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E28" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="G28" s="12" t="s">
         <v>196</v>
@@ -9024,22 +9020,22 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C29" s="13" t="s">
         <v>71</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E29" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="G29" s="12" t="s">
         <v>197</v>
@@ -9047,191 +9043,191 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C30" s="13" t="s">
         <v>71</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E30" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="G30" s="12" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C31" s="13" t="s">
         <v>71</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E31" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F31" s="12" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="G31" s="12" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C32" s="13" t="s">
         <v>71</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E32" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="G32" s="12" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C33" s="13" t="s">
         <v>71</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E33" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F33" s="12" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="G33" s="12" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C34" s="13" t="s">
         <v>71</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E34" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G34" s="12" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C35" s="13" t="s">
         <v>71</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E35" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="G35" s="12" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C36" s="13" t="s">
         <v>71</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E36" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F36" s="12" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="G36" s="12" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C37" s="13" t="s">
         <v>71</v>
       </c>
       <c r="D37" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E37" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F37" s="12" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="G37" s="12" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B38" s="12" t="s">
         <v>198</v>
@@ -9240,21 +9236,21 @@
         <v>71</v>
       </c>
       <c r="D38" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E38" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F38" s="12" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="G38" s="12" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B39" s="12" t="s">
         <v>199</v>
@@ -9263,21 +9259,21 @@
         <v>71</v>
       </c>
       <c r="D39" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E39" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F39" s="12" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="G39" s="12" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B40" s="12" t="s">
         <v>200</v>
@@ -9286,21 +9282,21 @@
         <v>71</v>
       </c>
       <c r="D40" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E40" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F40" s="12" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="G40" s="12" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B41" s="12" t="s">
         <v>201</v>
@@ -9309,21 +9305,21 @@
         <v>71</v>
       </c>
       <c r="D41" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E41" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F41" s="12" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="G41" s="12" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B42" s="12" t="s">
         <v>202</v>
@@ -9332,21 +9328,21 @@
         <v>71</v>
       </c>
       <c r="D42" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E42" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F42" s="12" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="G42" s="12" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B43" s="12" t="s">
         <v>203</v>
@@ -9355,21 +9351,21 @@
         <v>71</v>
       </c>
       <c r="D43" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E43" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F43" s="12" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="G43" s="12" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B44" s="12" t="s">
         <v>204</v>
@@ -9378,21 +9374,21 @@
         <v>71</v>
       </c>
       <c r="D44" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E44" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F44" s="12" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="G44" s="12" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B45" s="12" t="s">
         <v>205</v>
@@ -9401,21 +9397,21 @@
         <v>71</v>
       </c>
       <c r="D45" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E45" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F45" s="12" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="G45" s="12" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B46" s="12" t="s">
         <v>206</v>
@@ -9424,21 +9420,21 @@
         <v>71</v>
       </c>
       <c r="D46" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E46" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F46" s="12" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="G46" s="12" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B47" s="12" t="s">
         <v>207</v>
@@ -9447,21 +9443,21 @@
         <v>71</v>
       </c>
       <c r="D47" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E47" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F47" s="12" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="G47" s="12" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B48" s="12" t="s">
         <v>208</v>
@@ -9470,21 +9466,21 @@
         <v>71</v>
       </c>
       <c r="D48" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E48" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F48" s="12" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="G48" s="12" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B49" s="12" t="s">
         <v>209</v>
@@ -9493,21 +9489,21 @@
         <v>71</v>
       </c>
       <c r="D49" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E49" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F49" s="12" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="G49" s="12" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B50" s="12" t="s">
         <v>210</v>
@@ -9516,21 +9512,21 @@
         <v>71</v>
       </c>
       <c r="D50" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E50" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F50" s="12" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="G50" s="12" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B51" s="12" t="s">
         <v>211</v>
@@ -9539,21 +9535,21 @@
         <v>71</v>
       </c>
       <c r="D51" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E51" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F51" s="12" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="G51" s="12" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B52" s="12" t="s">
         <v>212</v>
@@ -9562,21 +9558,21 @@
         <v>71</v>
       </c>
       <c r="D52" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E52" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F52" s="12" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="G52" s="12" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B53" s="12" t="s">
         <v>213</v>
@@ -9585,21 +9581,21 @@
         <v>71</v>
       </c>
       <c r="D53" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E53" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F53" s="12" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="G53" s="12" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B54" s="12" t="s">
         <v>214</v>
@@ -9608,21 +9604,21 @@
         <v>71</v>
       </c>
       <c r="D54" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E54" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F54" s="12" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="G54" s="12" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B55" s="12" t="s">
         <v>215</v>
@@ -9631,21 +9627,21 @@
         <v>71</v>
       </c>
       <c r="D55" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E55" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F55" s="12" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="G55" s="12" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B56" s="12" t="s">
         <v>216</v>
@@ -9654,21 +9650,21 @@
         <v>71</v>
       </c>
       <c r="D56" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E56" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F56" s="12" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="G56" s="12" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="57" spans="1:7">
       <c r="A57" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B57" s="12" t="s">
         <v>217</v>
@@ -9677,21 +9673,21 @@
         <v>71</v>
       </c>
       <c r="D57" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E57" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F57" s="12" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="G57" s="12" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c r="A58" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B58" s="12" t="s">
         <v>218</v>
@@ -9700,21 +9696,21 @@
         <v>71</v>
       </c>
       <c r="D58" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E58" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F58" s="12" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="G58" s="12" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="59" spans="1:7">
       <c r="A59" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B59" s="12" t="s">
         <v>219</v>
@@ -9723,21 +9719,21 @@
         <v>71</v>
       </c>
       <c r="D59" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E59" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F59" s="12" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="G59" s="12" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c r="A60" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B60" s="12" t="s">
         <v>220</v>
@@ -9746,21 +9742,21 @@
         <v>71</v>
       </c>
       <c r="D60" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E60" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F60" s="12" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="G60" s="12" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c r="A61" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B61" s="12" t="s">
         <v>221</v>
@@ -9769,21 +9765,21 @@
         <v>71</v>
       </c>
       <c r="D61" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E61" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F61" s="12" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="G61" s="12" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="A62" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B62" s="12" t="s">
         <v>222</v>
@@ -9792,21 +9788,21 @@
         <v>71</v>
       </c>
       <c r="D62" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E62" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F62" s="12" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="G62" s="12" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="63" spans="1:7">
       <c r="A63" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B63" s="12" t="s">
         <v>223</v>
@@ -9815,21 +9811,21 @@
         <v>71</v>
       </c>
       <c r="D63" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E63" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F63" s="12" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="G63" s="12" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="64" spans="1:7">
       <c r="A64" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B64" s="12" t="s">
         <v>224</v>
@@ -9838,21 +9834,21 @@
         <v>71</v>
       </c>
       <c r="D64" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E64" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F64" s="12" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="G64" s="12" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="65" spans="1:7">
       <c r="A65" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B65" s="12" t="s">
         <v>225</v>
@@ -9861,21 +9857,21 @@
         <v>71</v>
       </c>
       <c r="D65" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E65" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F65" s="12" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="G65" s="12" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="66" spans="1:7">
       <c r="A66" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B66" s="12" t="s">
         <v>226</v>
@@ -9884,21 +9880,21 @@
         <v>71</v>
       </c>
       <c r="D66" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E66" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F66" s="12" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="G66" s="12" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="67" spans="1:7">
       <c r="A67" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B67" s="12" t="s">
         <v>227</v>
@@ -9907,21 +9903,21 @@
         <v>71</v>
       </c>
       <c r="D67" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E67" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F67" s="12" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="G67" s="12" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="68" spans="1:7">
       <c r="A68" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B68" s="12" t="s">
         <v>228</v>
@@ -9930,21 +9926,21 @@
         <v>71</v>
       </c>
       <c r="D68" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E68" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F68" s="12" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="G68" s="12" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="69" spans="1:7">
       <c r="A69" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B69" s="12" t="s">
         <v>229</v>
@@ -9953,21 +9949,21 @@
         <v>71</v>
       </c>
       <c r="D69" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E69" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F69" s="12" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="G69" s="12" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="70" spans="1:7">
       <c r="A70" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B70" s="12" t="s">
         <v>230</v>
@@ -9976,21 +9972,21 @@
         <v>71</v>
       </c>
       <c r="D70" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E70" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F70" s="12" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="G70" s="12" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="71" spans="1:7">
       <c r="A71" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B71" s="12" t="s">
         <v>231</v>
@@ -9999,21 +9995,21 @@
         <v>71</v>
       </c>
       <c r="D71" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E71" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F71" s="12" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="G71" s="12" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="72" spans="1:7">
       <c r="A72" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B72" s="12" t="s">
         <v>232</v>
@@ -10022,21 +10018,21 @@
         <v>71</v>
       </c>
       <c r="D72" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E72" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F72" s="12" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="G72" s="12" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="73" spans="1:7">
       <c r="A73" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B73" s="12" t="s">
         <v>233</v>
@@ -10045,246 +10041,246 @@
         <v>71</v>
       </c>
       <c r="D73" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E73" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F73" s="12" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="G73" s="12" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="74" spans="1:7">
       <c r="A74" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B74" s="12" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C74" s="13" t="s">
         <v>71</v>
       </c>
       <c r="D74" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E74" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F74" s="12" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="G74" s="12" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="75" spans="1:7">
       <c r="A75" s="13" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B75" s="12" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C75" s="13" t="s">
         <v>71</v>
       </c>
       <c r="D75" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E75" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F75" s="12" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="G75" s="12" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="76" spans="1:7">
       <c r="A76" s="13" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B76" s="12" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C76" s="13" t="s">
         <v>71</v>
       </c>
       <c r="D76" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E76" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F76" s="12" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="G76" s="12" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="77" spans="1:7">
       <c r="A77" s="13" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B77" s="12" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C77" s="13" t="s">
         <v>71</v>
       </c>
       <c r="D77" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E77" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F77" s="12" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="G77" s="12" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="78" spans="1:7">
       <c r="A78" s="13" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B78" s="12" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C78" s="13" t="s">
         <v>71</v>
       </c>
       <c r="D78" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E78" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F78" s="12" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="G78" s="12" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="79" spans="1:7">
       <c r="A79" s="13" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B79" s="12" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C79" s="13" t="s">
         <v>71</v>
       </c>
       <c r="D79" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E79" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F79" s="12" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="G79" s="12" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="80" spans="1:7">
       <c r="A80" s="13" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B80" s="12" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C80" s="13" t="s">
         <v>71</v>
       </c>
       <c r="D80" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E80" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F80" s="12" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="G80" s="12" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="81" spans="1:7">
       <c r="A81" s="13" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B81" s="12" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C81" s="13" t="s">
         <v>71</v>
       </c>
       <c r="D81" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E81" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F81" s="12" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="G81" s="12" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="82" spans="1:7">
       <c r="A82" s="13" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B82" s="12" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C82" s="13" t="s">
         <v>71</v>
       </c>
       <c r="D82" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E82" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F82" s="12" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="G82" s="12" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="83" spans="1:7">
       <c r="A83" s="13" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B83" s="12" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C83" s="13" t="s">
         <v>71</v>
       </c>
       <c r="D83" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E83" s="13" t="s">
         <v>73</v>
       </c>
       <c r="F83" s="12" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="G83" s="12" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="84" spans="1:7">

</xml_diff>